<commit_message>
Implemented ability to read Excel custom property to associate spec with file
</commit_message>
<xml_diff>
--- a/src/test/xlsTestFiles/test-assignments.xlsx
+++ b/src/test/xlsTestFiles/test-assignments.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/justin/Desktop/coding/xlsUploader/src/test/xlsTestFiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEF50402-745C-1A47-A508-3C954B78075A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{222C8125-2C97-E04E-9742-438DF4A6C337}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" xr2:uid="{B474F3A5-C3F8-2345-A3DB-673EF3609AE0}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:A1048576"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>